<commit_message>
Updated figure ordering in script and data sheet. Added figure s2.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="figure_2_8" sheetId="1" state="visible" r:id="rId2"/>
@@ -78,12 +78,6 @@
     <t xml:space="preserve">mølle</t>
   </si>
   <si>
-    <t xml:space="preserve">June-Aug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sep-May</t>
-  </si>
-  <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
@@ -142,6 +136,12 @@
   </si>
   <si>
     <t xml:space="preserve">log_chl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June-Aug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sep-May</t>
   </si>
   <si>
     <t xml:space="preserve">time</t>
@@ -287,11 +287,11 @@
   </sheetPr>
   <dimension ref="A1:G250"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5513,7 +5513,7 @@
       <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6368,221 +6368,423 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="topLeft" activeCell="R19" activeCellId="0" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>1.8</v>
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="n">
+        <v>79.6073933709307</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>9.87455204843373</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>4.921177909441</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>33.8656595791224</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>4.89126511165319</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>16.2490019776409</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>8.28030341844061</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>4.39268718966932</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>40.1331070589445</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>6.11753410551034</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>4.48243571159655</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>56.3441146201475</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>11.0700454367839</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>4.62204052351228</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>92.5279519093421</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>2.66705775701376</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>2.35772602743795</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>147.171996261618</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>6.01784858730663</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>8.23047790508636</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>5.56924032395773</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>13.6598012527773</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>22.3219487249751</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>13.201657181145</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>29.8856635613253</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>99.4843156419338</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>6.13747098910537</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>8.67851125880934</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>12.8455827836533</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0.611280097586474</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>94.3583718757015</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0.810191648205271</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>79.0436316995644</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="n">
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>163.063688340685</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>153.131596250255</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>5.96800513410482</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>134.25858343396</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>93.5217531531533</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>2.89653557970374</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>106.44013225886</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>74.3391242283898</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>2.9963020725472</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>60.6196909252294</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>29.1891051051926</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>31.1692737928745</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>147.171996261618</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>123.330762958152</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>2.60719040118546</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>57.5373342475814</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>68.9710216025141</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>6.21721779793854</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>289</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>345</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>277</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>276</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>225</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>163</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1" t="n">
-        <v>262</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>165</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1" t="n">
-        <v>193</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>167</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>160</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B17" s="1" t="n">
-        <v>176</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="n">
-        <v>181</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B19" s="1" t="n">
-        <v>197</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>210</v>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>134.25858343396</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>146.178703516115</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>1.13983231339495</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>229.79784783779</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>3.97490162749475</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -6601,423 +6803,1066 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>2.30535136944662</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>2.20682587603185</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0.525044807036845</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>2.2148438480477</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>2.18752072083646</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0.776701183988411</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C4" s="1" t="n">
+        <v>1.90308998699194</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.99563519459755</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0.69284691927723</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>2.21218760440396</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1.52504480703685</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0.499687082618404</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>2.22271647114758</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1.63042787502502</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>1.04532297878666</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>2.10720996964787</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1.82216807936802</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>1.02530586526477</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>2.00432137378264</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1.8318697742805</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0.89209460269048</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>2.00432137378264</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>1.82930377283102</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0.919078092376074</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>2.41161970596323</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>2.40312052117582</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0.447158031342219</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>2.43136376415899</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>2.31386722036915</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>0.462397997898956</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>2.13033376849501</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>1.9731278535997</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>0.462397997898956</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>1.53147891704226</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0.690196080028514</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>1.21218760440396</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0.919078092376074</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0.643452676486187</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>1.60530504614111</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>1.49692964807321</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0.929418925714293</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>1.51719589794997</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>2.43296929087441</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>2.39619934709574</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>0.079181246047625</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>2.09691001300806</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>1.95279244304409</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>0.653212513775344</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>2.02938377768521</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>1.8733206018154</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>0.477121254719662</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>2.05690485133647</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>1.95616843047536</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>0.761927838420529</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>2.14612803567824</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>2.07554696139253</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>-0.148741651280925</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>2.05307844348342</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>1.45788189673399</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>0.574031267727719</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>2.02118929906994</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>1.39794000867204</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>0.617000341120899</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>1.86805636182304</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>1.70671778233676</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>0.575187844927661</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>1.83314711191279</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>1.76566855475901</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>0.514547752660286</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>1.94694327069783</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>1.89872518158949</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>0.614897216033135</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>1.41497334797082</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>1.22530928172586</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>1.61023417533439</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>1.78461729263288</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>1.46686762035411</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>1.49540556314619</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>1.74585519517373</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>1.43136376415899</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>1.50379068305718</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>0.787460474518415</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>0.652246341003323</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>1.75281643118827</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>1.04532297878666</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>0.665580991017953</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>1.96848294855394</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B31" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>0.426511261364575</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>0.372912002970107</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>2.17026171539496</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>2.16136800223497</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>1.93094903116752</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>1.20139712432045</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>2.06818586174616</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>1.96894968098134</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>0.232996110392154</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>2.17026171539496</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>2.09342168516224</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>0.416640507338281</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>0.780317312140151</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>0.916453948549925</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>0.746634198937579</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>1.7664128471124</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>1.65513843481138</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>0.850646235183067</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>1.76192783842053</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>1.84073323461181</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <v>0.79448804665917</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="B38" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>1.13672056715641</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>1.35024801833416</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>1.12188798510368</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>2.62634036737504</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>2.73158876518674</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>0.037426497940624</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B40" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>2.49276038902684</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>2.62634036737504</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>-0.119186407719209</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B41" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>2.20682587603185</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>2.22010808804005</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>0.05307844348342</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>2.13033376849501</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>2.16731733474818</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>0.056904851336473</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>1.47712125471966</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>0.788875115775417</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>1.06069784035361</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>0.924279286061882</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <v>1.65609820201283</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="n">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="B45" s="1" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>0.740362689494244</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>0.832508912706236</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <v>1.65801139665711</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>1.23044892137827</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>0.866877814337499</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <v>1.73239375982297</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>2.25527250510331</v>
+      </c>
+      <c r="D47" s="1" t="n">
+        <v>2.24303804868629</v>
+      </c>
+      <c r="E47" s="1" t="n">
+        <v>0.155336037465062</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>1.84695532501982</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>1.70243053644553</v>
+      </c>
+      <c r="E48" s="1" t="n">
+        <v>0.679427896612119</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B49" s="1" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>1.13033376849501</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>0.740362689494244</v>
+      </c>
+      <c r="E49" s="1" t="n">
+        <v>2.19562294358694</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B50" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>1.48855071650044</v>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>1.35602585719312</v>
+      </c>
+      <c r="E50" s="1" t="n">
+        <v>1.69897000433602</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B51" s="1" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>1.19865708695442</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>0.117271295655764</v>
+      </c>
+      <c r="E51" s="1" t="n">
+        <v>2.23044892137827</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="B52" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>1.80482067872116</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>1.26245108973043</v>
+      </c>
+      <c r="E52" s="1" t="n">
+        <v>1.73158876518674</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B53" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>2.0899051114394</v>
+      </c>
+      <c r="D53" s="1" t="n">
+        <v>1.90633504180509</v>
+      </c>
+      <c r="E53" s="1" t="n">
+        <v>0.673020907128896</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B54" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>1.26951294421792</v>
+      </c>
+      <c r="D54" s="1" t="n">
+        <v>1.49554433754645</v>
+      </c>
+      <c r="E54" s="1" t="n">
+        <v>1.74115159885179</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="B55" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>79.6073933709307</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>9.87455204843373</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>4.921177909441</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>33.8656595791224</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>4.89126511165319</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>16.2490019776409</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>8.28030341844061</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>4.39268718966932</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>40.1331070589445</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>6.11753410551034</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>4.48243571159655</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>56.3441146201475</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>11.0700454367839</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>4.62204052351228</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>92.5279519093421</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>2.66705775701376</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>2.35772602743795</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>147.171996261618</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>6.01784858730663</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>8.23047790508636</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>5.56924032395773</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>13.6598012527773</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>22.3219487249751</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>13.201657181145</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>29.8856635613253</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>99.4843156419338</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>6.13747098910537</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>8.67851125880934</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>12.8455827836533</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>0.611280097586474</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>94.3583718757015</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>0.810191648205271</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>79.0436316995644</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="C55" s="1" t="n">
+        <v>0.65991620006985</v>
+      </c>
+      <c r="D55" s="1" t="n">
+        <v>0.980911937776844</v>
+      </c>
+      <c r="E55" s="1" t="n">
+        <v>1.51321760006794</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>0.631443769013172</v>
+      </c>
+      <c r="D56" s="1" t="n">
+        <v>0.978180516937414</v>
+      </c>
+      <c r="E56" s="1" t="n">
+        <v>1.71933128698373</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>163.063688340685</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>153.131596250255</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>5.96800513410482</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>134.25858343396</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>93.5217531531533</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>2.89653557970374</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>106.44013225886</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>74.3391242283898</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>2.9963020725472</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>60.6196909252294</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>29.1891051051926</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>31.1692737928745</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <v>147.171996261618</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>123.330762958152</v>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>2.60719040118546</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>57.5373342475814</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>68.9710216025141</v>
-      </c>
-      <c r="E22" s="1" t="n">
-        <v>6.21721779793854</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>134.25858343396</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>146.178703516115</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>1.13983231339495</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="1" t="n">
-        <v>229.79784783779</v>
-      </c>
-      <c r="E24" s="1" t="n">
-        <v>3.97490162749475</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="1" t="n">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>7</v>
+      <c r="B57" s="1" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>0.502427119984433</v>
+      </c>
+      <c r="D57" s="1" t="n">
+        <v>0.958085848521085</v>
+      </c>
+      <c r="E57" s="1" t="n">
+        <v>1.72835378202123</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="B58" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>0.829946695941636</v>
+      </c>
+      <c r="D58" s="1" t="n">
+        <v>1.14612803567824</v>
+      </c>
+      <c r="E58" s="1" t="n">
+        <v>1.568201724067</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B59" s="1" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>1.11727129565576</v>
+      </c>
+      <c r="D59" s="1" t="n">
+        <v>1.32014628611105</v>
+      </c>
+      <c r="E59" s="1" t="n">
+        <v>1.45939248775923</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="B60" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>1.55022835305509</v>
+      </c>
+      <c r="D60" s="1" t="n">
+        <v>1.40654018043396</v>
+      </c>
+      <c r="E60" s="1" t="n">
+        <v>1.47421626407626</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B61" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>1.90525604874845</v>
+      </c>
+      <c r="D61" s="1" t="n">
+        <v>1.68930885912362</v>
+      </c>
+      <c r="E61" s="1" t="n">
+        <v>0.477121254719662</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B62" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C62" s="1" t="n">
+        <v>2.04532297878666</v>
+      </c>
+      <c r="D62" s="1" t="n">
+        <v>1.97772360528885</v>
+      </c>
+      <c r="E62" s="1" t="n">
+        <v>0.923761960828701</v>
       </c>
     </row>
   </sheetData>
@@ -7036,1066 +7881,221 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T5" activeCellId="0" sqref="T5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>15</v>
+        <v>1.8</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>2.30535136944662</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>2.20682587603185</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>0.525044807036845</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>2.2148438480477</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>2.18752072083646</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>0.776701183988411</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1.90308998699194</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>0.99563519459755</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>0.69284691927723</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>17.5</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>2.21218760440396</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>1.52504480703685</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0.499687082618404</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>17</v>
+        <v>289</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>2.22271647114758</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>1.63042787502502</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>1.04532297878666</v>
+        <v>390</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>14</v>
+        <v>345</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>2.10720996964787</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>1.82216807936802</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>1.02530586526477</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>14.5</v>
+        <v>277</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>2.00432137378264</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>1.8318697742805</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>0.89209460269048</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>14</v>
+        <v>276</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>2.00432137378264</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>1.82930377283102</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>0.919078092376074</v>
+        <v>342</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>10.5</v>
+        <v>0</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>12</v>
+        <v>225</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>2.41161970596323</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>2.40312052117582</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>0.447158031342219</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>11.5</v>
+        <v>163</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>2.43136376415899</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>2.31386722036915</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>0.462397997898956</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>11.5</v>
+        <v>262</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>2.13033376849501</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>1.9731278535997</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>0.462397997898956</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>19</v>
+        <v>165</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>1.53147891704226</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>0.690196080028514</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>1.21218760440396</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>17.5</v>
+        <v>0</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>18.6</v>
+        <v>193</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>0.919078092376074</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>0.643452676486187</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>1.60530504614111</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>19</v>
+        <v>167</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>1.49692964807321</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>0.929418925714293</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>1.51719589794997</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>12</v>
+        <v>160</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>2.43296929087441</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>2.39619934709574</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>0.079181246047625</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>11.5</v>
+        <v>0</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>13</v>
+        <v>176</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>2.09691001300806</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>1.95279244304409</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>0.653212513775344</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>11.5</v>
+        <v>0</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>13.5</v>
+        <v>181</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>2.02938377768521</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>1.8733206018154</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>0.477121254719662</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>10</v>
+        <v>197</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>2.05690485133647</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>1.95616843047536</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>0.761927838420529</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1" t="n">
-        <v>10.5</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <v>2.14612803567824</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>2.07554696139253</v>
-      </c>
-      <c r="E20" s="1" t="n">
-        <v>-0.148741651280925</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B21" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <v>2.05307844348342</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>1.45788189673399</v>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>0.574031267727719</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B22" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>2.02118929906994</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>1.39794000867204</v>
-      </c>
-      <c r="E22" s="1" t="n">
-        <v>0.617000341120899</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="B23" s="1" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>1.86805636182304</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>1.70671778233676</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>0.575187844927661</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="B24" s="1" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="C24" s="1" t="n">
-        <v>1.83314711191279</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>1.76566855475901</v>
-      </c>
-      <c r="E24" s="1" t="n">
-        <v>0.514547752660286</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B25" s="1" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="C25" s="1" t="n">
-        <v>1.94694327069783</v>
-      </c>
-      <c r="D25" s="1" t="n">
-        <v>1.89872518158949</v>
-      </c>
-      <c r="E25" s="1" t="n">
-        <v>0.614897216033135</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="B26" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <v>1.41497334797082</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>1.22530928172586</v>
-      </c>
-      <c r="E26" s="1" t="n">
-        <v>1.61023417533439</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="B27" s="1" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>1.78461729263288</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>1.46686762035411</v>
-      </c>
-      <c r="E27" s="1" t="n">
-        <v>1.49540556314619</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="B28" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="C28" s="1" t="n">
-        <v>1.74585519517373</v>
-      </c>
-      <c r="D28" s="1" t="n">
-        <v>1.43136376415899</v>
-      </c>
-      <c r="E28" s="1" t="n">
-        <v>1.50379068305718</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>15.5</v>
-      </c>
-      <c r="B29" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="C29" s="1" t="n">
-        <v>0.787460474518415</v>
-      </c>
-      <c r="D29" s="1" t="n">
-        <v>0.652246341003323</v>
-      </c>
-      <c r="E29" s="1" t="n">
-        <v>1.75281643118827</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B30" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="C30" s="1" t="n">
-        <v>1.04532297878666</v>
-      </c>
-      <c r="D30" s="1" t="n">
-        <v>0.665580991017953</v>
-      </c>
-      <c r="E30" s="1" t="n">
-        <v>1.96848294855394</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B31" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="C31" s="1" t="n">
-        <v>0.426511261364575</v>
-      </c>
-      <c r="D31" s="1" t="n">
-        <v>0.372912002970107</v>
-      </c>
-      <c r="E31" s="1" t="n">
-        <v>2.17026171539496</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B32" s="1" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <v>2.16136800223497</v>
-      </c>
-      <c r="D32" s="1" t="n">
-        <v>1.93094903116752</v>
-      </c>
-      <c r="E32" s="1" t="n">
-        <v>1.20139712432045</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B33" s="1" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="C33" s="1" t="n">
-        <v>2.06818586174616</v>
-      </c>
-      <c r="D33" s="1" t="n">
-        <v>1.96894968098134</v>
-      </c>
-      <c r="E33" s="1" t="n">
-        <v>0.232996110392154</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="B34" s="1" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="C34" s="1" t="n">
-        <v>2.17026171539496</v>
-      </c>
-      <c r="D34" s="1" t="n">
-        <v>2.09342168516224</v>
-      </c>
-      <c r="E34" s="1" t="n">
-        <v>0.416640507338281</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B35" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="C35" s="1" t="n">
-        <v>0.780317312140151</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <v>0.916453948549925</v>
-      </c>
-      <c r="E35" s="1" t="n">
-        <v>0.746634198937579</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>10.5</v>
-      </c>
-      <c r="B36" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="C36" s="1" t="n">
-        <v>1.7664128471124</v>
-      </c>
-      <c r="D36" s="1" t="n">
-        <v>1.65513843481138</v>
-      </c>
-      <c r="E36" s="1" t="n">
-        <v>0.850646235183067</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B37" s="1" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="C37" s="1" t="n">
-        <v>1.76192783842053</v>
-      </c>
-      <c r="D37" s="1" t="n">
-        <v>1.84073323461181</v>
-      </c>
-      <c r="E37" s="1" t="n">
-        <v>0.79448804665917</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>19.5</v>
-      </c>
-      <c r="B38" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>1.13672056715641</v>
-      </c>
-      <c r="D38" s="1" t="n">
-        <v>1.35024801833416</v>
-      </c>
-      <c r="E38" s="1" t="n">
-        <v>1.12188798510368</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B39" s="1" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="C39" s="1" t="n">
-        <v>2.62634036737504</v>
-      </c>
-      <c r="D39" s="1" t="n">
-        <v>2.73158876518674</v>
-      </c>
-      <c r="E39" s="1" t="n">
-        <v>0.037426497940624</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B40" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="C40" s="1" t="n">
-        <v>2.49276038902684</v>
-      </c>
-      <c r="D40" s="1" t="n">
-        <v>2.62634036737504</v>
-      </c>
-      <c r="E40" s="1" t="n">
-        <v>-0.119186407719209</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B41" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>2.20682587603185</v>
-      </c>
-      <c r="D41" s="1" t="n">
-        <v>2.22010808804005</v>
-      </c>
-      <c r="E41" s="1" t="n">
-        <v>0.05307844348342</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B42" s="1" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="C42" s="1" t="n">
-        <v>2.13033376849501</v>
-      </c>
-      <c r="D42" s="1" t="n">
-        <v>2.16731733474818</v>
-      </c>
-      <c r="E42" s="1" t="n">
-        <v>0.056904851336473</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B43" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="C43" s="1" t="n">
-        <v>1.47712125471966</v>
-      </c>
-      <c r="D43" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E43" s="1" t="n">
-        <v>0.788875115775417</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B44" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="C44" s="1" t="n">
-        <v>1.06069784035361</v>
-      </c>
-      <c r="D44" s="1" t="n">
-        <v>0.924279286061882</v>
-      </c>
-      <c r="E44" s="1" t="n">
-        <v>1.65609820201283</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B45" s="1" t="n">
-        <v>19.5</v>
-      </c>
-      <c r="C45" s="1" t="n">
-        <v>0.740362689494244</v>
-      </c>
-      <c r="D45" s="1" t="n">
-        <v>0.832508912706236</v>
-      </c>
-      <c r="E45" s="1" t="n">
-        <v>1.65801139665711</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
-        <v>20.5</v>
-      </c>
-      <c r="B46" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="C46" s="1" t="n">
-        <v>1.23044892137827</v>
-      </c>
-      <c r="D46" s="1" t="n">
-        <v>0.866877814337499</v>
-      </c>
-      <c r="E46" s="1" t="n">
-        <v>1.73239375982297</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="B47" s="1" t="n">
-        <v>15.5</v>
-      </c>
-      <c r="C47" s="1" t="n">
-        <v>2.25527250510331</v>
-      </c>
-      <c r="D47" s="1" t="n">
-        <v>2.24303804868629</v>
-      </c>
-      <c r="E47" s="1" t="n">
-        <v>0.155336037465062</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B48" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="C48" s="1" t="n">
-        <v>1.84695532501982</v>
-      </c>
-      <c r="D48" s="1" t="n">
-        <v>1.70243053644553</v>
-      </c>
-      <c r="E48" s="1" t="n">
-        <v>0.679427896612119</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B49" s="1" t="n">
-        <v>17.5</v>
-      </c>
-      <c r="C49" s="1" t="n">
-        <v>1.13033376849501</v>
-      </c>
-      <c r="D49" s="1" t="n">
-        <v>0.740362689494244</v>
-      </c>
-      <c r="E49" s="1" t="n">
-        <v>2.19562294358694</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B50" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="C50" s="1" t="n">
-        <v>1.48855071650044</v>
-      </c>
-      <c r="D50" s="1" t="n">
-        <v>1.35602585719312</v>
-      </c>
-      <c r="E50" s="1" t="n">
-        <v>1.69897000433602</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B51" s="1" t="n">
-        <v>19.5</v>
-      </c>
-      <c r="C51" s="1" t="n">
-        <v>1.19865708695442</v>
-      </c>
-      <c r="D51" s="1" t="n">
-        <v>0.117271295655764</v>
-      </c>
-      <c r="E51" s="1" t="n">
-        <v>2.23044892137827</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
-        <v>20.5</v>
-      </c>
-      <c r="B52" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <v>1.80482067872116</v>
-      </c>
-      <c r="D52" s="1" t="n">
-        <v>1.26245108973043</v>
-      </c>
-      <c r="E52" s="1" t="n">
-        <v>1.73158876518674</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B53" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="C53" s="1" t="n">
-        <v>2.0899051114394</v>
-      </c>
-      <c r="D53" s="1" t="n">
-        <v>1.90633504180509</v>
-      </c>
-      <c r="E53" s="1" t="n">
-        <v>0.673020907128896</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B54" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="C54" s="1" t="n">
-        <v>1.26951294421792</v>
-      </c>
-      <c r="D54" s="1" t="n">
-        <v>1.49554433754645</v>
-      </c>
-      <c r="E54" s="1" t="n">
-        <v>1.74115159885179</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
-        <v>21.5</v>
-      </c>
-      <c r="B55" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="C55" s="1" t="n">
-        <v>0.65991620006985</v>
-      </c>
-      <c r="D55" s="1" t="n">
-        <v>0.980911937776844</v>
-      </c>
-      <c r="E55" s="1" t="n">
-        <v>1.51321760006794</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B56" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="C56" s="1" t="n">
-        <v>0.631443769013172</v>
-      </c>
-      <c r="D56" s="1" t="n">
-        <v>0.978180516937414</v>
-      </c>
-      <c r="E56" s="1" t="n">
-        <v>1.71933128698373</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B57" s="1" t="n">
-        <v>19.5</v>
-      </c>
-      <c r="C57" s="1" t="n">
-        <v>0.502427119984433</v>
-      </c>
-      <c r="D57" s="1" t="n">
-        <v>0.958085848521085</v>
-      </c>
-      <c r="E57" s="1" t="n">
-        <v>1.72835378202123</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
-        <v>21.5</v>
-      </c>
-      <c r="B58" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="C58" s="1" t="n">
-        <v>0.829946695941636</v>
-      </c>
-      <c r="D58" s="1" t="n">
-        <v>1.14612803567824</v>
-      </c>
-      <c r="E58" s="1" t="n">
-        <v>1.568201724067</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B59" s="1" t="n">
-        <v>20.5</v>
-      </c>
-      <c r="C59" s="1" t="n">
-        <v>1.11727129565576</v>
-      </c>
-      <c r="D59" s="1" t="n">
-        <v>1.32014628611105</v>
-      </c>
-      <c r="E59" s="1" t="n">
-        <v>1.45939248775923</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
-        <v>20.5</v>
-      </c>
-      <c r="B60" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="C60" s="1" t="n">
-        <v>1.55022835305509</v>
-      </c>
-      <c r="D60" s="1" t="n">
-        <v>1.40654018043396</v>
-      </c>
-      <c r="E60" s="1" t="n">
-        <v>1.47421626407626</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B61" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="C61" s="1" t="n">
-        <v>1.90525604874845</v>
-      </c>
-      <c r="D61" s="1" t="n">
-        <v>1.68930885912362</v>
-      </c>
-      <c r="E61" s="1" t="n">
-        <v>0.477121254719662</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B62" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="C62" s="1" t="n">
-        <v>2.04532297878666</v>
-      </c>
-      <c r="D62" s="1" t="n">
-        <v>1.97772360528885</v>
-      </c>
-      <c r="E62" s="1" t="n">
-        <v>0.923761960828701</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -8120,7 +8120,7 @@
       <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>